<commit_message>
Structuring Dysarthric Models F02
</commit_message>
<xml_diff>
--- a/Dysarthric Speakers.xlsx
+++ b/Dysarthric Speakers.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dhvan\Documents\GitHub\P4P-Transformer-ASR-for-Dysarthric-Speech\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B05DEE6-F986-4C0B-90D5-67AE3A2D5E01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E711FE1-5386-4DA9-AA49-93F58642C6E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{65B8B18D-9A80-4269-9189-9F5DDA7ECA5A}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" activeTab="1" xr2:uid="{65B8B18D-9A80-4269-9189-9F5DDA7ECA5A}"/>
   </bookViews>
   <sheets>
-    <sheet name="F02" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="M04" sheetId="3" r:id="rId1"/>
+    <sheet name="F02" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="41">
   <si>
     <t>Model Name</t>
   </si>
@@ -189,15 +190,103 @@
     <t>F03_T3+D1</t>
   </si>
   <si>
-    <t>F03_Dense</t>
-  </si>
-  <si>
     <t>&lt;__main__.DisplayOutputs object at 0x7fba881604f0&gt;</t>
   </si>
   <si>
-    <t>Token Embeddings
-+
-Dense</t>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Speaker:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> M04</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Intelligibility:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Very Low</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Speech Vision Accuracy:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 10.94</t>
+    </r>
+  </si>
+  <si>
+    <t>M04_E1.h5</t>
+  </si>
+  <si>
+    <t>M04_E12.h5</t>
+  </si>
+  <si>
+    <t>M04_E123</t>
+  </si>
+  <si>
+    <t>M04_E1234</t>
+  </si>
+  <si>
+    <t>M04_E12345</t>
+  </si>
+  <si>
+    <t>M04_TE</t>
+  </si>
+  <si>
+    <t>M04_T3+D123</t>
+  </si>
+  <si>
+    <t>M04_T3+D12</t>
+  </si>
+  <si>
+    <t>M04_T3+D1</t>
   </si>
 </sst>
 </file>
@@ -336,7 +425,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -354,18 +443,12 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -377,12 +460,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2722,11 +2819,1151 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5C52428-6FF2-4AC0-9F9B-B62B85A25342}">
+  <dimension ref="A1:J94"/>
+  <sheetViews>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="12.86328125" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" customWidth="1"/>
+    <col min="4" max="4" width="13.9296875" customWidth="1"/>
+    <col min="7" max="7" width="20.19921875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="15"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="9"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A6" s="3"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="10"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A7" s="3"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="10"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A8" s="3"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="10"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A9" s="3"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="10"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A10" s="3"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="10"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A11" s="3"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="10"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A12" s="3"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="10"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A13" s="4"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="11"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A14" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="9"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A15" s="3"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="10"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A16" s="3"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="10"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A17" s="3"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="10"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A18" s="3"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="10"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A19" s="3"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="10"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A20" s="3"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="10"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A21" s="3"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="10"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A22" s="4"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="11"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A23" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="9"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A24" s="3"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="10"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A25" s="3"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="10"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A26" s="3"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="10"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A27" s="3"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="10"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A28" s="3"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="10"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A29" s="3"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="10"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A30" s="3"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="6"/>
+      <c r="I30" s="10"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A31" s="4"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="7"/>
+      <c r="I31" s="11"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A32" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C32" s="8"/>
+      <c r="D32" s="8"/>
+      <c r="E32" s="8"/>
+      <c r="F32" s="8"/>
+      <c r="G32" s="8"/>
+      <c r="H32" s="8"/>
+      <c r="I32" s="9"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A33" s="3"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="6"/>
+      <c r="I33" s="10"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A34" s="3"/>
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="6"/>
+      <c r="H34" s="6"/>
+      <c r="I34" s="10"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A35" s="3"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="6"/>
+      <c r="H35" s="6"/>
+      <c r="I35" s="10"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A36" s="3"/>
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="6"/>
+      <c r="G36" s="6"/>
+      <c r="H36" s="6"/>
+      <c r="I36" s="10"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A37" s="3"/>
+      <c r="B37" s="6"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="6"/>
+      <c r="G37" s="6"/>
+      <c r="H37" s="6"/>
+      <c r="I37" s="10"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A38" s="3"/>
+      <c r="B38" s="6"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="6"/>
+      <c r="G38" s="6"/>
+      <c r="H38" s="6"/>
+      <c r="I38" s="10"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A39" s="3"/>
+      <c r="B39" s="6"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="6"/>
+      <c r="G39" s="6"/>
+      <c r="H39" s="6"/>
+      <c r="I39" s="10"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A40" s="4"/>
+      <c r="B40" s="7"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="7"/>
+      <c r="F40" s="7"/>
+      <c r="G40" s="7"/>
+      <c r="H40" s="7"/>
+      <c r="I40" s="11"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A41" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C41" s="8"/>
+      <c r="D41" s="8"/>
+      <c r="E41" s="8"/>
+      <c r="F41" s="8"/>
+      <c r="G41" s="8"/>
+      <c r="H41" s="8"/>
+      <c r="I41" s="9"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A42" s="3"/>
+      <c r="B42" s="6"/>
+      <c r="C42" s="6"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="6"/>
+      <c r="F42" s="6"/>
+      <c r="G42" s="6"/>
+      <c r="H42" s="6"/>
+      <c r="I42" s="10"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A43" s="3"/>
+      <c r="B43" s="6"/>
+      <c r="C43" s="6"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="6"/>
+      <c r="F43" s="6"/>
+      <c r="G43" s="6"/>
+      <c r="H43" s="6"/>
+      <c r="I43" s="10"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A44" s="3"/>
+      <c r="B44" s="6"/>
+      <c r="C44" s="6"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="6"/>
+      <c r="F44" s="6"/>
+      <c r="G44" s="6"/>
+      <c r="H44" s="6"/>
+      <c r="I44" s="10"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A45" s="3"/>
+      <c r="B45" s="6"/>
+      <c r="C45" s="6"/>
+      <c r="D45" s="6"/>
+      <c r="E45" s="6"/>
+      <c r="F45" s="6"/>
+      <c r="G45" s="6"/>
+      <c r="H45" s="6"/>
+      <c r="I45" s="10"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A46" s="3"/>
+      <c r="B46" s="6"/>
+      <c r="C46" s="6"/>
+      <c r="D46" s="6"/>
+      <c r="E46" s="6"/>
+      <c r="F46" s="6"/>
+      <c r="G46" s="6"/>
+      <c r="H46" s="6"/>
+      <c r="I46" s="10"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A47" s="3"/>
+      <c r="B47" s="6"/>
+      <c r="C47" s="6"/>
+      <c r="D47" s="6"/>
+      <c r="E47" s="6"/>
+      <c r="F47" s="6"/>
+      <c r="G47" s="6"/>
+      <c r="H47" s="6"/>
+      <c r="I47" s="10"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A48" s="3"/>
+      <c r="B48" s="6"/>
+      <c r="C48" s="6"/>
+      <c r="D48" s="6"/>
+      <c r="E48" s="6"/>
+      <c r="F48" s="6"/>
+      <c r="G48" s="6"/>
+      <c r="H48" s="6"/>
+      <c r="I48" s="10"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A49" s="4"/>
+      <c r="B49" s="7"/>
+      <c r="C49" s="7"/>
+      <c r="D49" s="7"/>
+      <c r="E49" s="7"/>
+      <c r="F49" s="7"/>
+      <c r="G49" s="7"/>
+      <c r="H49" s="7"/>
+      <c r="I49" s="11"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A50" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C50" s="8"/>
+      <c r="D50" s="8"/>
+      <c r="E50" s="8"/>
+      <c r="F50" s="8"/>
+      <c r="G50" s="8"/>
+      <c r="H50" s="8"/>
+      <c r="I50" s="9"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A51" s="3"/>
+      <c r="B51" s="12"/>
+      <c r="C51" s="6"/>
+      <c r="D51" s="6"/>
+      <c r="E51" s="6"/>
+      <c r="F51" s="6"/>
+      <c r="G51" s="6"/>
+      <c r="H51" s="6"/>
+      <c r="I51" s="10"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A52" s="3"/>
+      <c r="B52" s="12"/>
+      <c r="C52" s="6"/>
+      <c r="D52" s="6"/>
+      <c r="E52" s="6"/>
+      <c r="F52" s="6"/>
+      <c r="G52" s="6"/>
+      <c r="H52" s="6"/>
+      <c r="I52" s="10"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A53" s="3"/>
+      <c r="B53" s="12"/>
+      <c r="C53" s="6"/>
+      <c r="D53" s="6"/>
+      <c r="E53" s="6"/>
+      <c r="F53" s="6"/>
+      <c r="G53" s="6"/>
+      <c r="H53" s="6"/>
+      <c r="I53" s="10"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A54" s="3"/>
+      <c r="B54" s="12"/>
+      <c r="C54" s="6"/>
+      <c r="D54" s="6"/>
+      <c r="E54" s="6"/>
+      <c r="F54" s="6"/>
+      <c r="G54" s="6"/>
+      <c r="H54" s="6"/>
+      <c r="I54" s="10"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A55" s="3"/>
+      <c r="B55" s="12"/>
+      <c r="C55" s="6"/>
+      <c r="D55" s="6"/>
+      <c r="E55" s="6"/>
+      <c r="F55" s="6"/>
+      <c r="G55" s="6"/>
+      <c r="H55" s="6"/>
+      <c r="I55" s="10"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A56" s="3"/>
+      <c r="B56" s="12"/>
+      <c r="C56" s="6"/>
+      <c r="D56" s="6"/>
+      <c r="E56" s="6"/>
+      <c r="F56" s="6"/>
+      <c r="G56" s="6"/>
+      <c r="H56" s="6"/>
+      <c r="I56" s="10"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A57" s="3"/>
+      <c r="B57" s="12"/>
+      <c r="C57" s="6"/>
+      <c r="D57" s="6"/>
+      <c r="E57" s="6"/>
+      <c r="F57" s="6"/>
+      <c r="G57" s="6"/>
+      <c r="H57" s="6"/>
+      <c r="I57" s="10"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A58" s="4"/>
+      <c r="B58" s="13"/>
+      <c r="C58" s="7"/>
+      <c r="D58" s="7"/>
+      <c r="E58" s="7"/>
+      <c r="F58" s="7"/>
+      <c r="G58" s="7"/>
+      <c r="H58" s="7"/>
+      <c r="I58" s="11"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A59" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C59" s="8"/>
+      <c r="D59" s="8"/>
+      <c r="E59" s="8"/>
+      <c r="F59" s="8"/>
+      <c r="G59" s="8"/>
+      <c r="H59" s="8"/>
+      <c r="I59" s="9"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A60" s="3"/>
+      <c r="B60" s="12"/>
+      <c r="C60" s="6"/>
+      <c r="D60" s="6"/>
+      <c r="E60" s="6"/>
+      <c r="F60" s="6"/>
+      <c r="G60" s="6"/>
+      <c r="H60" s="6"/>
+      <c r="I60" s="10"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A61" s="3"/>
+      <c r="B61" s="12"/>
+      <c r="C61" s="6"/>
+      <c r="D61" s="6"/>
+      <c r="E61" s="6"/>
+      <c r="F61" s="6"/>
+      <c r="G61" s="6"/>
+      <c r="H61" s="6"/>
+      <c r="I61" s="10"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A62" s="3"/>
+      <c r="B62" s="12"/>
+      <c r="C62" s="6"/>
+      <c r="D62" s="6"/>
+      <c r="E62" s="6"/>
+      <c r="F62" s="6"/>
+      <c r="G62" s="6"/>
+      <c r="H62" s="6"/>
+      <c r="I62" s="10"/>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A63" s="3"/>
+      <c r="B63" s="12"/>
+      <c r="C63" s="6"/>
+      <c r="D63" s="6"/>
+      <c r="E63" s="6"/>
+      <c r="F63" s="6"/>
+      <c r="G63" s="6"/>
+      <c r="H63" s="6"/>
+      <c r="I63" s="10"/>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A64" s="3"/>
+      <c r="B64" s="12"/>
+      <c r="C64" s="6"/>
+      <c r="D64" s="6"/>
+      <c r="E64" s="6"/>
+      <c r="F64" s="6"/>
+      <c r="G64" s="6"/>
+      <c r="H64" s="6"/>
+      <c r="I64" s="10"/>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A65" s="3"/>
+      <c r="B65" s="12"/>
+      <c r="C65" s="6"/>
+      <c r="D65" s="6"/>
+      <c r="E65" s="6"/>
+      <c r="F65" s="6"/>
+      <c r="G65" s="6"/>
+      <c r="H65" s="6"/>
+      <c r="I65" s="10"/>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A66" s="3"/>
+      <c r="B66" s="12"/>
+      <c r="C66" s="6"/>
+      <c r="D66" s="6"/>
+      <c r="E66" s="6"/>
+      <c r="F66" s="6"/>
+      <c r="G66" s="6"/>
+      <c r="H66" s="6"/>
+      <c r="I66" s="10"/>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A67" s="4"/>
+      <c r="B67" s="13"/>
+      <c r="C67" s="7"/>
+      <c r="D67" s="7"/>
+      <c r="E67" s="7"/>
+      <c r="F67" s="7"/>
+      <c r="G67" s="7"/>
+      <c r="H67" s="7"/>
+      <c r="I67" s="11"/>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A68" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C68" s="8"/>
+      <c r="D68" s="8"/>
+      <c r="E68" s="8"/>
+      <c r="F68" s="8"/>
+      <c r="G68" s="8"/>
+      <c r="H68" s="8"/>
+      <c r="I68" s="9"/>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A69" s="3"/>
+      <c r="B69" s="6"/>
+      <c r="C69" s="6"/>
+      <c r="D69" s="6"/>
+      <c r="E69" s="6"/>
+      <c r="F69" s="6"/>
+      <c r="G69" s="6"/>
+      <c r="H69" s="6"/>
+      <c r="I69" s="10"/>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A70" s="3"/>
+      <c r="B70" s="6"/>
+      <c r="C70" s="6"/>
+      <c r="D70" s="6"/>
+      <c r="E70" s="6"/>
+      <c r="F70" s="6"/>
+      <c r="G70" s="6"/>
+      <c r="H70" s="6"/>
+      <c r="I70" s="10"/>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A71" s="3"/>
+      <c r="B71" s="6"/>
+      <c r="C71" s="6"/>
+      <c r="D71" s="6"/>
+      <c r="E71" s="6"/>
+      <c r="F71" s="6"/>
+      <c r="G71" s="6"/>
+      <c r="H71" s="6"/>
+      <c r="I71" s="10"/>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A72" s="3"/>
+      <c r="B72" s="6"/>
+      <c r="C72" s="6"/>
+      <c r="D72" s="6"/>
+      <c r="E72" s="6"/>
+      <c r="F72" s="6"/>
+      <c r="G72" s="6"/>
+      <c r="H72" s="6"/>
+      <c r="I72" s="10"/>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A73" s="3"/>
+      <c r="B73" s="6"/>
+      <c r="C73" s="6"/>
+      <c r="D73" s="6"/>
+      <c r="E73" s="6"/>
+      <c r="F73" s="6"/>
+      <c r="G73" s="6"/>
+      <c r="H73" s="6"/>
+      <c r="I73" s="10"/>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A74" s="3"/>
+      <c r="B74" s="6"/>
+      <c r="C74" s="6"/>
+      <c r="D74" s="6"/>
+      <c r="E74" s="6"/>
+      <c r="F74" s="6"/>
+      <c r="G74" s="6"/>
+      <c r="H74" s="6"/>
+      <c r="I74" s="10"/>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A75" s="3"/>
+      <c r="B75" s="6"/>
+      <c r="C75" s="6"/>
+      <c r="D75" s="6"/>
+      <c r="E75" s="6"/>
+      <c r="F75" s="6"/>
+      <c r="G75" s="6"/>
+      <c r="H75" s="6"/>
+      <c r="I75" s="10"/>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A76" s="4"/>
+      <c r="B76" s="7"/>
+      <c r="C76" s="7"/>
+      <c r="D76" s="7"/>
+      <c r="E76" s="7"/>
+      <c r="F76" s="7"/>
+      <c r="G76" s="7"/>
+      <c r="H76" s="7"/>
+      <c r="I76" s="11"/>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A77" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B77" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C77" s="8"/>
+      <c r="D77" s="8"/>
+      <c r="E77" s="8"/>
+      <c r="F77" s="8"/>
+      <c r="G77" s="8"/>
+      <c r="H77" s="8"/>
+      <c r="I77" s="9"/>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A78" s="3"/>
+      <c r="B78" s="20"/>
+      <c r="C78" s="20"/>
+      <c r="D78" s="20"/>
+      <c r="E78" s="20"/>
+      <c r="F78" s="20"/>
+      <c r="G78" s="20"/>
+      <c r="H78" s="20"/>
+      <c r="I78" s="10"/>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A79" s="3"/>
+      <c r="B79" s="20"/>
+      <c r="C79" s="20"/>
+      <c r="D79" s="20"/>
+      <c r="E79" s="20"/>
+      <c r="F79" s="20"/>
+      <c r="G79" s="20"/>
+      <c r="H79" s="20"/>
+      <c r="I79" s="10"/>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A80" s="3"/>
+      <c r="B80" s="20"/>
+      <c r="C80" s="20"/>
+      <c r="D80" s="20"/>
+      <c r="E80" s="20"/>
+      <c r="F80" s="20"/>
+      <c r="G80" s="20"/>
+      <c r="H80" s="20"/>
+      <c r="I80" s="10"/>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A81" s="3"/>
+      <c r="B81" s="20"/>
+      <c r="C81" s="20"/>
+      <c r="D81" s="20"/>
+      <c r="E81" s="20"/>
+      <c r="F81" s="20"/>
+      <c r="G81" s="20"/>
+      <c r="H81" s="20"/>
+      <c r="I81" s="10"/>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A82" s="3"/>
+      <c r="B82" s="20"/>
+      <c r="C82" s="20"/>
+      <c r="D82" s="20"/>
+      <c r="E82" s="20"/>
+      <c r="F82" s="20"/>
+      <c r="G82" s="20"/>
+      <c r="H82" s="20"/>
+      <c r="I82" s="10"/>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A83" s="3"/>
+      <c r="B83" s="20"/>
+      <c r="C83" s="20"/>
+      <c r="D83" s="20"/>
+      <c r="E83" s="20"/>
+      <c r="F83" s="20"/>
+      <c r="G83" s="20"/>
+      <c r="H83" s="20"/>
+      <c r="I83" s="10"/>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A84" s="3"/>
+      <c r="B84" s="20"/>
+      <c r="C84" s="20"/>
+      <c r="D84" s="20"/>
+      <c r="E84" s="20"/>
+      <c r="F84" s="20"/>
+      <c r="G84" s="20"/>
+      <c r="H84" s="20"/>
+      <c r="I84" s="10"/>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A85" s="4"/>
+      <c r="B85" s="7"/>
+      <c r="C85" s="7"/>
+      <c r="D85" s="7"/>
+      <c r="E85" s="7"/>
+      <c r="F85" s="7"/>
+      <c r="G85" s="7"/>
+      <c r="H85" s="7"/>
+      <c r="I85" s="11"/>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A86" s="19"/>
+      <c r="B86" s="21"/>
+      <c r="C86" s="19"/>
+      <c r="D86" s="19"/>
+      <c r="E86" s="19"/>
+      <c r="F86" s="19"/>
+      <c r="G86" s="19"/>
+      <c r="H86" s="19"/>
+      <c r="I86" s="19"/>
+      <c r="J86" s="18"/>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A87" s="19"/>
+      <c r="B87" s="19"/>
+      <c r="C87" s="19"/>
+      <c r="D87" s="19"/>
+      <c r="E87" s="19"/>
+      <c r="F87" s="19"/>
+      <c r="G87" s="19"/>
+      <c r="H87" s="19"/>
+      <c r="I87" s="19"/>
+      <c r="J87" s="18"/>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A88" s="19"/>
+      <c r="B88" s="19"/>
+      <c r="C88" s="19"/>
+      <c r="D88" s="19"/>
+      <c r="E88" s="19"/>
+      <c r="F88" s="19"/>
+      <c r="G88" s="19"/>
+      <c r="H88" s="19"/>
+      <c r="I88" s="19"/>
+      <c r="J88" s="18"/>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A89" s="19"/>
+      <c r="B89" s="19"/>
+      <c r="C89" s="19"/>
+      <c r="D89" s="19"/>
+      <c r="E89" s="19"/>
+      <c r="F89" s="19"/>
+      <c r="G89" s="19"/>
+      <c r="H89" s="19"/>
+      <c r="I89" s="19"/>
+      <c r="J89" s="18"/>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A90" s="19"/>
+      <c r="B90" s="19"/>
+      <c r="C90" s="19"/>
+      <c r="D90" s="19"/>
+      <c r="E90" s="19"/>
+      <c r="F90" s="19"/>
+      <c r="G90" s="19"/>
+      <c r="H90" s="19"/>
+      <c r="I90" s="19"/>
+      <c r="J90" s="18"/>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A91" s="19"/>
+      <c r="B91" s="19"/>
+      <c r="C91" s="19"/>
+      <c r="D91" s="19"/>
+      <c r="E91" s="19"/>
+      <c r="F91" s="19"/>
+      <c r="G91" s="19"/>
+      <c r="H91" s="19"/>
+      <c r="I91" s="19"/>
+      <c r="J91" s="18"/>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A92" s="19"/>
+      <c r="B92" s="19"/>
+      <c r="C92" s="19"/>
+      <c r="D92" s="19"/>
+      <c r="E92" s="19"/>
+      <c r="F92" s="19"/>
+      <c r="G92" s="19"/>
+      <c r="H92" s="19"/>
+      <c r="I92" s="19"/>
+      <c r="J92" s="18"/>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A93" s="19"/>
+      <c r="B93" s="19"/>
+      <c r="C93" s="19"/>
+      <c r="D93" s="19"/>
+      <c r="E93" s="19"/>
+      <c r="F93" s="19"/>
+      <c r="G93" s="19"/>
+      <c r="H93" s="19"/>
+      <c r="I93" s="19"/>
+      <c r="J93" s="18"/>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A94" s="19"/>
+      <c r="B94" s="19"/>
+      <c r="C94" s="19"/>
+      <c r="D94" s="19"/>
+      <c r="E94" s="19"/>
+      <c r="F94" s="19"/>
+      <c r="G94" s="19"/>
+      <c r="H94" s="19"/>
+      <c r="I94" s="19"/>
+      <c r="J94" s="18"/>
+    </row>
+  </sheetData>
+  <mergeCells count="48">
+    <mergeCell ref="A68:A76"/>
+    <mergeCell ref="B68:B76"/>
+    <mergeCell ref="C68:C76"/>
+    <mergeCell ref="D68:F76"/>
+    <mergeCell ref="G68:I76"/>
+    <mergeCell ref="A77:A85"/>
+    <mergeCell ref="B77:B85"/>
+    <mergeCell ref="C77:C85"/>
+    <mergeCell ref="D77:F85"/>
+    <mergeCell ref="G77:I85"/>
+    <mergeCell ref="A50:A58"/>
+    <mergeCell ref="B50:B58"/>
+    <mergeCell ref="C50:C58"/>
+    <mergeCell ref="D50:F58"/>
+    <mergeCell ref="G50:I58"/>
+    <mergeCell ref="A59:A67"/>
+    <mergeCell ref="B59:B67"/>
+    <mergeCell ref="C59:C67"/>
+    <mergeCell ref="D59:F67"/>
+    <mergeCell ref="G59:I67"/>
+    <mergeCell ref="A32:A40"/>
+    <mergeCell ref="B32:B40"/>
+    <mergeCell ref="C32:C40"/>
+    <mergeCell ref="D32:F40"/>
+    <mergeCell ref="G32:I40"/>
+    <mergeCell ref="A41:A49"/>
+    <mergeCell ref="B41:B49"/>
+    <mergeCell ref="C41:C49"/>
+    <mergeCell ref="D41:F49"/>
+    <mergeCell ref="G41:I49"/>
+    <mergeCell ref="A14:A22"/>
+    <mergeCell ref="B14:B22"/>
+    <mergeCell ref="C14:C22"/>
+    <mergeCell ref="D14:F22"/>
+    <mergeCell ref="G14:I22"/>
+    <mergeCell ref="A23:A31"/>
+    <mergeCell ref="B23:B31"/>
+    <mergeCell ref="C23:C31"/>
+    <mergeCell ref="D23:F31"/>
+    <mergeCell ref="G23:I31"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="G4:I4"/>
+    <mergeCell ref="A5:A13"/>
+    <mergeCell ref="B5:B13"/>
+    <mergeCell ref="C5:C13"/>
+    <mergeCell ref="D5:F13"/>
+    <mergeCell ref="G5:I13"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{715F97D4-1A77-4245-8120-8092DD2AD5B3}">
-  <dimension ref="A1:I94"/>
+  <dimension ref="A1:J94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="68" workbookViewId="0">
-      <selection activeCell="B86" sqref="B86:B94"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="68" workbookViewId="0">
+      <selection activeCell="M87" sqref="M87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2745,10 +3982,10 @@
       <c r="B1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="14"/>
+      <c r="D1" s="15"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
@@ -2760,16 +3997,16 @@
       <c r="C4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="D4" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15" t="s">
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="15"/>
-      <c r="I4" s="15"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
@@ -2787,95 +4024,95 @@
       <c r="F5" s="8"/>
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
-      <c r="I5" s="11"/>
+      <c r="I5" s="9"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" s="3"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="12"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="10"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" s="3"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="12"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="10"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8" s="3"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="12"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="10"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9" s="3"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="12"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="10"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10" s="3"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="12"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="10"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11" s="3"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="12"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="10"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12" s="3"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="12"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="10"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A13" s="4"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="13"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="11"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14" s="2" t="s">
@@ -2893,95 +4130,95 @@
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
       <c r="H14" s="8"/>
-      <c r="I14" s="11"/>
+      <c r="I14" s="9"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A15" s="3"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="12"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="10"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A16" s="3"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="12"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="10"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A17" s="3"/>
-      <c r="B17" s="9"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="12"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="10"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A18" s="3"/>
-      <c r="B18" s="9"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="12"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="10"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A19" s="3"/>
-      <c r="B19" s="9"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="12"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="10"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A20" s="3"/>
-      <c r="B20" s="9"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="12"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="10"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A21" s="3"/>
-      <c r="B21" s="9"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="12"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="10"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A22" s="4"/>
-      <c r="B22" s="10"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="10"/>
-      <c r="I22" s="13"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="11"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A23" s="2" t="s">
@@ -2999,101 +4236,101 @@
       <c r="F23" s="8"/>
       <c r="G23" s="8"/>
       <c r="H23" s="8"/>
-      <c r="I23" s="11"/>
+      <c r="I23" s="9"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A24" s="3"/>
-      <c r="B24" s="9"/>
-      <c r="C24" s="9"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
-      <c r="H24" s="9"/>
-      <c r="I24" s="12"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="10"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A25" s="3"/>
-      <c r="B25" s="9"/>
-      <c r="C25" s="9"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="9"/>
-      <c r="G25" s="9"/>
-      <c r="H25" s="9"/>
-      <c r="I25" s="12"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="10"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A26" s="3"/>
-      <c r="B26" s="9"/>
-      <c r="C26" s="9"/>
-      <c r="D26" s="9"/>
-      <c r="E26" s="9"/>
-      <c r="F26" s="9"/>
-      <c r="G26" s="9"/>
-      <c r="H26" s="9"/>
-      <c r="I26" s="12"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="10"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A27" s="3"/>
-      <c r="B27" s="9"/>
-      <c r="C27" s="9"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="9"/>
-      <c r="F27" s="9"/>
-      <c r="G27" s="9"/>
-      <c r="H27" s="9"/>
-      <c r="I27" s="12"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="10"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A28" s="3"/>
-      <c r="B28" s="9"/>
-      <c r="C28" s="9"/>
-      <c r="D28" s="9"/>
-      <c r="E28" s="9"/>
-      <c r="F28" s="9"/>
-      <c r="G28" s="9"/>
-      <c r="H28" s="9"/>
-      <c r="I28" s="12"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="10"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A29" s="3"/>
-      <c r="B29" s="9"/>
-      <c r="C29" s="9"/>
-      <c r="D29" s="9"/>
-      <c r="E29" s="9"/>
-      <c r="F29" s="9"/>
-      <c r="G29" s="9"/>
-      <c r="H29" s="9"/>
-      <c r="I29" s="12"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="10"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A30" s="3"/>
-      <c r="B30" s="9"/>
-      <c r="C30" s="9"/>
-      <c r="D30" s="9"/>
-      <c r="E30" s="9"/>
-      <c r="F30" s="9"/>
-      <c r="G30" s="9"/>
-      <c r="H30" s="9"/>
-      <c r="I30" s="12"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="6"/>
+      <c r="I30" s="10"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A31" s="4"/>
-      <c r="B31" s="10"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="10"/>
-      <c r="E31" s="10"/>
-      <c r="F31" s="10"/>
-      <c r="G31" s="10"/>
-      <c r="H31" s="10"/>
-      <c r="I31" s="13"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="7"/>
+      <c r="I31" s="11"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A32" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B32" s="16" t="s">
+      <c r="B32" s="14" t="s">
         <v>16</v>
       </c>
       <c r="C32" s="8">
@@ -3105,95 +4342,95 @@
       <c r="F32" s="8"/>
       <c r="G32" s="8"/>
       <c r="H32" s="8"/>
-      <c r="I32" s="11"/>
+      <c r="I32" s="9"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A33" s="3"/>
-      <c r="B33" s="14"/>
-      <c r="C33" s="9"/>
-      <c r="D33" s="9"/>
-      <c r="E33" s="9"/>
-      <c r="F33" s="9"/>
-      <c r="G33" s="9"/>
-      <c r="H33" s="9"/>
-      <c r="I33" s="12"/>
+      <c r="B33" s="15"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="6"/>
+      <c r="I33" s="10"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A34" s="3"/>
-      <c r="B34" s="14"/>
-      <c r="C34" s="9"/>
-      <c r="D34" s="9"/>
-      <c r="E34" s="9"/>
-      <c r="F34" s="9"/>
-      <c r="G34" s="9"/>
-      <c r="H34" s="9"/>
-      <c r="I34" s="12"/>
+      <c r="B34" s="15"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="6"/>
+      <c r="H34" s="6"/>
+      <c r="I34" s="10"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A35" s="3"/>
-      <c r="B35" s="14"/>
-      <c r="C35" s="9"/>
-      <c r="D35" s="9"/>
-      <c r="E35" s="9"/>
-      <c r="F35" s="9"/>
-      <c r="G35" s="9"/>
-      <c r="H35" s="9"/>
-      <c r="I35" s="12"/>
+      <c r="B35" s="15"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="6"/>
+      <c r="H35" s="6"/>
+      <c r="I35" s="10"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A36" s="3"/>
-      <c r="B36" s="14"/>
-      <c r="C36" s="9"/>
-      <c r="D36" s="9"/>
-      <c r="E36" s="9"/>
-      <c r="F36" s="9"/>
-      <c r="G36" s="9"/>
-      <c r="H36" s="9"/>
-      <c r="I36" s="12"/>
+      <c r="B36" s="15"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="6"/>
+      <c r="G36" s="6"/>
+      <c r="H36" s="6"/>
+      <c r="I36" s="10"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A37" s="3"/>
-      <c r="B37" s="14"/>
-      <c r="C37" s="9"/>
-      <c r="D37" s="9"/>
-      <c r="E37" s="9"/>
-      <c r="F37" s="9"/>
-      <c r="G37" s="9"/>
-      <c r="H37" s="9"/>
-      <c r="I37" s="12"/>
+      <c r="B37" s="15"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="6"/>
+      <c r="G37" s="6"/>
+      <c r="H37" s="6"/>
+      <c r="I37" s="10"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A38" s="3"/>
-      <c r="B38" s="14"/>
-      <c r="C38" s="9"/>
-      <c r="D38" s="9"/>
-      <c r="E38" s="9"/>
-      <c r="F38" s="9"/>
-      <c r="G38" s="9"/>
-      <c r="H38" s="9"/>
-      <c r="I38" s="12"/>
+      <c r="B38" s="15"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="6"/>
+      <c r="G38" s="6"/>
+      <c r="H38" s="6"/>
+      <c r="I38" s="10"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A39" s="3"/>
-      <c r="B39" s="14"/>
-      <c r="C39" s="9"/>
-      <c r="D39" s="9"/>
-      <c r="E39" s="9"/>
-      <c r="F39" s="9"/>
-      <c r="G39" s="9"/>
-      <c r="H39" s="9"/>
-      <c r="I39" s="12"/>
+      <c r="B39" s="15"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="6"/>
+      <c r="G39" s="6"/>
+      <c r="H39" s="6"/>
+      <c r="I39" s="10"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A40" s="4"/>
-      <c r="B40" s="17"/>
-      <c r="C40" s="10"/>
-      <c r="D40" s="10"/>
-      <c r="E40" s="10"/>
-      <c r="F40" s="10"/>
-      <c r="G40" s="10"/>
-      <c r="H40" s="10"/>
-      <c r="I40" s="13"/>
+      <c r="B40" s="16"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="7"/>
+      <c r="F40" s="7"/>
+      <c r="G40" s="7"/>
+      <c r="H40" s="7"/>
+      <c r="I40" s="11"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A41" s="2" t="s">
@@ -3211,95 +4448,95 @@
       <c r="F41" s="8"/>
       <c r="G41" s="8"/>
       <c r="H41" s="8"/>
-      <c r="I41" s="11"/>
+      <c r="I41" s="9"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A42" s="3"/>
-      <c r="B42" s="9"/>
-      <c r="C42" s="9"/>
-      <c r="D42" s="9"/>
-      <c r="E42" s="9"/>
-      <c r="F42" s="9"/>
-      <c r="G42" s="9"/>
-      <c r="H42" s="9"/>
-      <c r="I42" s="12"/>
+      <c r="B42" s="6"/>
+      <c r="C42" s="6"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="6"/>
+      <c r="F42" s="6"/>
+      <c r="G42" s="6"/>
+      <c r="H42" s="6"/>
+      <c r="I42" s="10"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A43" s="3"/>
-      <c r="B43" s="9"/>
-      <c r="C43" s="9"/>
-      <c r="D43" s="9"/>
-      <c r="E43" s="9"/>
-      <c r="F43" s="9"/>
-      <c r="G43" s="9"/>
-      <c r="H43" s="9"/>
-      <c r="I43" s="12"/>
+      <c r="B43" s="6"/>
+      <c r="C43" s="6"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="6"/>
+      <c r="F43" s="6"/>
+      <c r="G43" s="6"/>
+      <c r="H43" s="6"/>
+      <c r="I43" s="10"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A44" s="3"/>
-      <c r="B44" s="9"/>
-      <c r="C44" s="9"/>
-      <c r="D44" s="9"/>
-      <c r="E44" s="9"/>
-      <c r="F44" s="9"/>
-      <c r="G44" s="9"/>
-      <c r="H44" s="9"/>
-      <c r="I44" s="12"/>
+      <c r="B44" s="6"/>
+      <c r="C44" s="6"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="6"/>
+      <c r="F44" s="6"/>
+      <c r="G44" s="6"/>
+      <c r="H44" s="6"/>
+      <c r="I44" s="10"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A45" s="3"/>
-      <c r="B45" s="9"/>
-      <c r="C45" s="9"/>
-      <c r="D45" s="9"/>
-      <c r="E45" s="9"/>
-      <c r="F45" s="9"/>
-      <c r="G45" s="9"/>
-      <c r="H45" s="9"/>
-      <c r="I45" s="12"/>
+      <c r="B45" s="6"/>
+      <c r="C45" s="6"/>
+      <c r="D45" s="6"/>
+      <c r="E45" s="6"/>
+      <c r="F45" s="6"/>
+      <c r="G45" s="6"/>
+      <c r="H45" s="6"/>
+      <c r="I45" s="10"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A46" s="3"/>
-      <c r="B46" s="9"/>
-      <c r="C46" s="9"/>
-      <c r="D46" s="9"/>
-      <c r="E46" s="9"/>
-      <c r="F46" s="9"/>
-      <c r="G46" s="9"/>
-      <c r="H46" s="9"/>
-      <c r="I46" s="12"/>
+      <c r="B46" s="6"/>
+      <c r="C46" s="6"/>
+      <c r="D46" s="6"/>
+      <c r="E46" s="6"/>
+      <c r="F46" s="6"/>
+      <c r="G46" s="6"/>
+      <c r="H46" s="6"/>
+      <c r="I46" s="10"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A47" s="3"/>
-      <c r="B47" s="9"/>
-      <c r="C47" s="9"/>
-      <c r="D47" s="9"/>
-      <c r="E47" s="9"/>
-      <c r="F47" s="9"/>
-      <c r="G47" s="9"/>
-      <c r="H47" s="9"/>
-      <c r="I47" s="12"/>
+      <c r="B47" s="6"/>
+      <c r="C47" s="6"/>
+      <c r="D47" s="6"/>
+      <c r="E47" s="6"/>
+      <c r="F47" s="6"/>
+      <c r="G47" s="6"/>
+      <c r="H47" s="6"/>
+      <c r="I47" s="10"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A48" s="3"/>
-      <c r="B48" s="9"/>
-      <c r="C48" s="9"/>
-      <c r="D48" s="9"/>
-      <c r="E48" s="9"/>
-      <c r="F48" s="9"/>
-      <c r="G48" s="9"/>
-      <c r="H48" s="9"/>
-      <c r="I48" s="12"/>
+      <c r="B48" s="6"/>
+      <c r="C48" s="6"/>
+      <c r="D48" s="6"/>
+      <c r="E48" s="6"/>
+      <c r="F48" s="6"/>
+      <c r="G48" s="6"/>
+      <c r="H48" s="6"/>
+      <c r="I48" s="10"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A49" s="4"/>
-      <c r="B49" s="10"/>
-      <c r="C49" s="10"/>
-      <c r="D49" s="10"/>
-      <c r="E49" s="10"/>
-      <c r="F49" s="10"/>
-      <c r="G49" s="10"/>
-      <c r="H49" s="10"/>
-      <c r="I49" s="13"/>
+      <c r="B49" s="7"/>
+      <c r="C49" s="7"/>
+      <c r="D49" s="7"/>
+      <c r="E49" s="7"/>
+      <c r="F49" s="7"/>
+      <c r="G49" s="7"/>
+      <c r="H49" s="7"/>
+      <c r="I49" s="11"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A50" s="2" t="s">
@@ -3317,95 +4554,95 @@
       <c r="F50" s="8"/>
       <c r="G50" s="8"/>
       <c r="H50" s="8"/>
-      <c r="I50" s="11"/>
+      <c r="I50" s="9"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A51" s="3"/>
-      <c r="B51" s="6"/>
-      <c r="C51" s="9"/>
-      <c r="D51" s="9"/>
-      <c r="E51" s="9"/>
-      <c r="F51" s="9"/>
-      <c r="G51" s="9"/>
-      <c r="H51" s="9"/>
-      <c r="I51" s="12"/>
+      <c r="B51" s="12"/>
+      <c r="C51" s="6"/>
+      <c r="D51" s="6"/>
+      <c r="E51" s="6"/>
+      <c r="F51" s="6"/>
+      <c r="G51" s="6"/>
+      <c r="H51" s="6"/>
+      <c r="I51" s="10"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A52" s="3"/>
-      <c r="B52" s="6"/>
-      <c r="C52" s="9"/>
-      <c r="D52" s="9"/>
-      <c r="E52" s="9"/>
-      <c r="F52" s="9"/>
-      <c r="G52" s="9"/>
-      <c r="H52" s="9"/>
-      <c r="I52" s="12"/>
+      <c r="B52" s="12"/>
+      <c r="C52" s="6"/>
+      <c r="D52" s="6"/>
+      <c r="E52" s="6"/>
+      <c r="F52" s="6"/>
+      <c r="G52" s="6"/>
+      <c r="H52" s="6"/>
+      <c r="I52" s="10"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A53" s="3"/>
-      <c r="B53" s="6"/>
-      <c r="C53" s="9"/>
-      <c r="D53" s="9"/>
-      <c r="E53" s="9"/>
-      <c r="F53" s="9"/>
-      <c r="G53" s="9"/>
-      <c r="H53" s="9"/>
-      <c r="I53" s="12"/>
+      <c r="B53" s="12"/>
+      <c r="C53" s="6"/>
+      <c r="D53" s="6"/>
+      <c r="E53" s="6"/>
+      <c r="F53" s="6"/>
+      <c r="G53" s="6"/>
+      <c r="H53" s="6"/>
+      <c r="I53" s="10"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A54" s="3"/>
-      <c r="B54" s="6"/>
-      <c r="C54" s="9"/>
-      <c r="D54" s="9"/>
-      <c r="E54" s="9"/>
-      <c r="F54" s="9"/>
-      <c r="G54" s="9"/>
-      <c r="H54" s="9"/>
-      <c r="I54" s="12"/>
+      <c r="B54" s="12"/>
+      <c r="C54" s="6"/>
+      <c r="D54" s="6"/>
+      <c r="E54" s="6"/>
+      <c r="F54" s="6"/>
+      <c r="G54" s="6"/>
+      <c r="H54" s="6"/>
+      <c r="I54" s="10"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A55" s="3"/>
-      <c r="B55" s="6"/>
-      <c r="C55" s="9"/>
-      <c r="D55" s="9"/>
-      <c r="E55" s="9"/>
-      <c r="F55" s="9"/>
-      <c r="G55" s="9"/>
-      <c r="H55" s="9"/>
-      <c r="I55" s="12"/>
+      <c r="B55" s="12"/>
+      <c r="C55" s="6"/>
+      <c r="D55" s="6"/>
+      <c r="E55" s="6"/>
+      <c r="F55" s="6"/>
+      <c r="G55" s="6"/>
+      <c r="H55" s="6"/>
+      <c r="I55" s="10"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A56" s="3"/>
-      <c r="B56" s="6"/>
-      <c r="C56" s="9"/>
-      <c r="D56" s="9"/>
-      <c r="E56" s="9"/>
-      <c r="F56" s="9"/>
-      <c r="G56" s="9"/>
-      <c r="H56" s="9"/>
-      <c r="I56" s="12"/>
+      <c r="B56" s="12"/>
+      <c r="C56" s="6"/>
+      <c r="D56" s="6"/>
+      <c r="E56" s="6"/>
+      <c r="F56" s="6"/>
+      <c r="G56" s="6"/>
+      <c r="H56" s="6"/>
+      <c r="I56" s="10"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A57" s="3"/>
-      <c r="B57" s="6"/>
-      <c r="C57" s="9"/>
-      <c r="D57" s="9"/>
-      <c r="E57" s="9"/>
-      <c r="F57" s="9"/>
-      <c r="G57" s="9"/>
-      <c r="H57" s="9"/>
-      <c r="I57" s="12"/>
+      <c r="B57" s="12"/>
+      <c r="C57" s="6"/>
+      <c r="D57" s="6"/>
+      <c r="E57" s="6"/>
+      <c r="F57" s="6"/>
+      <c r="G57" s="6"/>
+      <c r="H57" s="6"/>
+      <c r="I57" s="10"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A58" s="4"/>
-      <c r="B58" s="7"/>
-      <c r="C58" s="10"/>
-      <c r="D58" s="10"/>
-      <c r="E58" s="10"/>
-      <c r="F58" s="10"/>
-      <c r="G58" s="10"/>
-      <c r="H58" s="10"/>
-      <c r="I58" s="13"/>
+      <c r="B58" s="13"/>
+      <c r="C58" s="7"/>
+      <c r="D58" s="7"/>
+      <c r="E58" s="7"/>
+      <c r="F58" s="7"/>
+      <c r="G58" s="7"/>
+      <c r="H58" s="7"/>
+      <c r="I58" s="11"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A59" s="2" t="s">
@@ -3423,95 +4660,95 @@
       <c r="F59" s="8"/>
       <c r="G59" s="8"/>
       <c r="H59" s="8"/>
-      <c r="I59" s="11"/>
+      <c r="I59" s="9"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A60" s="3"/>
-      <c r="B60" s="6"/>
-      <c r="C60" s="9"/>
-      <c r="D60" s="9"/>
-      <c r="E60" s="9"/>
-      <c r="F60" s="9"/>
-      <c r="G60" s="9"/>
-      <c r="H60" s="9"/>
-      <c r="I60" s="12"/>
+      <c r="B60" s="12"/>
+      <c r="C60" s="6"/>
+      <c r="D60" s="6"/>
+      <c r="E60" s="6"/>
+      <c r="F60" s="6"/>
+      <c r="G60" s="6"/>
+      <c r="H60" s="6"/>
+      <c r="I60" s="10"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A61" s="3"/>
-      <c r="B61" s="6"/>
-      <c r="C61" s="9"/>
-      <c r="D61" s="9"/>
-      <c r="E61" s="9"/>
-      <c r="F61" s="9"/>
-      <c r="G61" s="9"/>
-      <c r="H61" s="9"/>
-      <c r="I61" s="12"/>
+      <c r="B61" s="12"/>
+      <c r="C61" s="6"/>
+      <c r="D61" s="6"/>
+      <c r="E61" s="6"/>
+      <c r="F61" s="6"/>
+      <c r="G61" s="6"/>
+      <c r="H61" s="6"/>
+      <c r="I61" s="10"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A62" s="3"/>
-      <c r="B62" s="6"/>
-      <c r="C62" s="9"/>
-      <c r="D62" s="9"/>
-      <c r="E62" s="9"/>
-      <c r="F62" s="9"/>
-      <c r="G62" s="9"/>
-      <c r="H62" s="9"/>
-      <c r="I62" s="12"/>
+      <c r="B62" s="12"/>
+      <c r="C62" s="6"/>
+      <c r="D62" s="6"/>
+      <c r="E62" s="6"/>
+      <c r="F62" s="6"/>
+      <c r="G62" s="6"/>
+      <c r="H62" s="6"/>
+      <c r="I62" s="10"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A63" s="3"/>
-      <c r="B63" s="6"/>
-      <c r="C63" s="9"/>
-      <c r="D63" s="9"/>
-      <c r="E63" s="9"/>
-      <c r="F63" s="9"/>
-      <c r="G63" s="9"/>
-      <c r="H63" s="9"/>
-      <c r="I63" s="12"/>
+      <c r="B63" s="12"/>
+      <c r="C63" s="6"/>
+      <c r="D63" s="6"/>
+      <c r="E63" s="6"/>
+      <c r="F63" s="6"/>
+      <c r="G63" s="6"/>
+      <c r="H63" s="6"/>
+      <c r="I63" s="10"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A64" s="3"/>
-      <c r="B64" s="6"/>
-      <c r="C64" s="9"/>
-      <c r="D64" s="9"/>
-      <c r="E64" s="9"/>
-      <c r="F64" s="9"/>
-      <c r="G64" s="9"/>
-      <c r="H64" s="9"/>
-      <c r="I64" s="12"/>
+      <c r="B64" s="12"/>
+      <c r="C64" s="6"/>
+      <c r="D64" s="6"/>
+      <c r="E64" s="6"/>
+      <c r="F64" s="6"/>
+      <c r="G64" s="6"/>
+      <c r="H64" s="6"/>
+      <c r="I64" s="10"/>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A65" s="3"/>
-      <c r="B65" s="6"/>
-      <c r="C65" s="9"/>
-      <c r="D65" s="9"/>
-      <c r="E65" s="9"/>
-      <c r="F65" s="9"/>
-      <c r="G65" s="9"/>
-      <c r="H65" s="9"/>
-      <c r="I65" s="12"/>
+      <c r="B65" s="12"/>
+      <c r="C65" s="6"/>
+      <c r="D65" s="6"/>
+      <c r="E65" s="6"/>
+      <c r="F65" s="6"/>
+      <c r="G65" s="6"/>
+      <c r="H65" s="6"/>
+      <c r="I65" s="10"/>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A66" s="3"/>
-      <c r="B66" s="6"/>
-      <c r="C66" s="9"/>
-      <c r="D66" s="9"/>
-      <c r="E66" s="9"/>
-      <c r="F66" s="9"/>
-      <c r="G66" s="9"/>
-      <c r="H66" s="9"/>
-      <c r="I66" s="12"/>
+      <c r="B66" s="12"/>
+      <c r="C66" s="6"/>
+      <c r="D66" s="6"/>
+      <c r="E66" s="6"/>
+      <c r="F66" s="6"/>
+      <c r="G66" s="6"/>
+      <c r="H66" s="6"/>
+      <c r="I66" s="10"/>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A67" s="4"/>
-      <c r="B67" s="7"/>
-      <c r="C67" s="10"/>
-      <c r="D67" s="10"/>
-      <c r="E67" s="10"/>
-      <c r="F67" s="10"/>
-      <c r="G67" s="10"/>
-      <c r="H67" s="10"/>
-      <c r="I67" s="13"/>
+      <c r="B67" s="13"/>
+      <c r="C67" s="7"/>
+      <c r="D67" s="7"/>
+      <c r="E67" s="7"/>
+      <c r="F67" s="7"/>
+      <c r="G67" s="7"/>
+      <c r="H67" s="7"/>
+      <c r="I67" s="11"/>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A68" s="2" t="s">
@@ -3528,95 +4765,95 @@
       <c r="F68" s="8"/>
       <c r="G68" s="8"/>
       <c r="H68" s="8"/>
-      <c r="I68" s="11"/>
+      <c r="I68" s="9"/>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A69" s="3"/>
-      <c r="B69" s="9"/>
-      <c r="C69" s="9"/>
-      <c r="D69" s="9"/>
-      <c r="E69" s="9"/>
-      <c r="F69" s="9"/>
-      <c r="G69" s="9"/>
-      <c r="H69" s="9"/>
-      <c r="I69" s="12"/>
+      <c r="B69" s="6"/>
+      <c r="C69" s="6"/>
+      <c r="D69" s="6"/>
+      <c r="E69" s="6"/>
+      <c r="F69" s="6"/>
+      <c r="G69" s="6"/>
+      <c r="H69" s="6"/>
+      <c r="I69" s="10"/>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A70" s="3"/>
-      <c r="B70" s="9"/>
-      <c r="C70" s="9"/>
-      <c r="D70" s="9"/>
-      <c r="E70" s="9"/>
-      <c r="F70" s="9"/>
-      <c r="G70" s="9"/>
-      <c r="H70" s="9"/>
-      <c r="I70" s="12"/>
+      <c r="B70" s="6"/>
+      <c r="C70" s="6"/>
+      <c r="D70" s="6"/>
+      <c r="E70" s="6"/>
+      <c r="F70" s="6"/>
+      <c r="G70" s="6"/>
+      <c r="H70" s="6"/>
+      <c r="I70" s="10"/>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A71" s="3"/>
-      <c r="B71" s="9"/>
-      <c r="C71" s="9"/>
-      <c r="D71" s="9"/>
-      <c r="E71" s="9"/>
-      <c r="F71" s="9"/>
-      <c r="G71" s="9"/>
-      <c r="H71" s="9"/>
-      <c r="I71" s="12"/>
+      <c r="B71" s="6"/>
+      <c r="C71" s="6"/>
+      <c r="D71" s="6"/>
+      <c r="E71" s="6"/>
+      <c r="F71" s="6"/>
+      <c r="G71" s="6"/>
+      <c r="H71" s="6"/>
+      <c r="I71" s="10"/>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A72" s="3"/>
-      <c r="B72" s="9"/>
-      <c r="C72" s="9"/>
-      <c r="D72" s="9"/>
-      <c r="E72" s="9"/>
-      <c r="F72" s="9"/>
-      <c r="G72" s="9"/>
-      <c r="H72" s="9"/>
-      <c r="I72" s="12"/>
+      <c r="B72" s="6"/>
+      <c r="C72" s="6"/>
+      <c r="D72" s="6"/>
+      <c r="E72" s="6"/>
+      <c r="F72" s="6"/>
+      <c r="G72" s="6"/>
+      <c r="H72" s="6"/>
+      <c r="I72" s="10"/>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A73" s="3"/>
-      <c r="B73" s="9"/>
-      <c r="C73" s="9"/>
-      <c r="D73" s="9"/>
-      <c r="E73" s="9"/>
-      <c r="F73" s="9"/>
-      <c r="G73" s="9"/>
-      <c r="H73" s="9"/>
-      <c r="I73" s="12"/>
+      <c r="B73" s="6"/>
+      <c r="C73" s="6"/>
+      <c r="D73" s="6"/>
+      <c r="E73" s="6"/>
+      <c r="F73" s="6"/>
+      <c r="G73" s="6"/>
+      <c r="H73" s="6"/>
+      <c r="I73" s="10"/>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A74" s="3"/>
-      <c r="B74" s="9"/>
-      <c r="C74" s="9"/>
-      <c r="D74" s="9"/>
-      <c r="E74" s="9"/>
-      <c r="F74" s="9"/>
-      <c r="G74" s="9"/>
-      <c r="H74" s="9"/>
-      <c r="I74" s="12"/>
+      <c r="B74" s="6"/>
+      <c r="C74" s="6"/>
+      <c r="D74" s="6"/>
+      <c r="E74" s="6"/>
+      <c r="F74" s="6"/>
+      <c r="G74" s="6"/>
+      <c r="H74" s="6"/>
+      <c r="I74" s="10"/>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A75" s="3"/>
-      <c r="B75" s="9"/>
-      <c r="C75" s="9"/>
-      <c r="D75" s="9"/>
-      <c r="E75" s="9"/>
-      <c r="F75" s="9"/>
-      <c r="G75" s="9"/>
-      <c r="H75" s="9"/>
-      <c r="I75" s="12"/>
+      <c r="B75" s="6"/>
+      <c r="C75" s="6"/>
+      <c r="D75" s="6"/>
+      <c r="E75" s="6"/>
+      <c r="F75" s="6"/>
+      <c r="G75" s="6"/>
+      <c r="H75" s="6"/>
+      <c r="I75" s="10"/>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A76" s="4"/>
-      <c r="B76" s="10"/>
-      <c r="C76" s="10"/>
-      <c r="D76" s="10"/>
-      <c r="E76" s="10"/>
-      <c r="F76" s="10"/>
-      <c r="G76" s="10"/>
-      <c r="H76" s="10"/>
-      <c r="I76" s="13"/>
+      <c r="B76" s="7"/>
+      <c r="C76" s="7"/>
+      <c r="D76" s="7"/>
+      <c r="E76" s="7"/>
+      <c r="F76" s="7"/>
+      <c r="G76" s="7"/>
+      <c r="H76" s="7"/>
+      <c r="I76" s="11"/>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A77" s="2" t="s">
@@ -3633,231 +4870,221 @@
       <c r="F77" s="8"/>
       <c r="G77" s="8"/>
       <c r="H77" s="8"/>
-      <c r="I77" s="11"/>
+      <c r="I77" s="9"/>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A78" s="3"/>
-      <c r="B78" s="9"/>
-      <c r="C78" s="9"/>
-      <c r="D78" s="9"/>
-      <c r="E78" s="9"/>
-      <c r="F78" s="9"/>
-      <c r="G78" s="9"/>
-      <c r="H78" s="9"/>
-      <c r="I78" s="12"/>
+      <c r="B78" s="20"/>
+      <c r="C78" s="20"/>
+      <c r="D78" s="20"/>
+      <c r="E78" s="20"/>
+      <c r="F78" s="20"/>
+      <c r="G78" s="20"/>
+      <c r="H78" s="20"/>
+      <c r="I78" s="10"/>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A79" s="3"/>
-      <c r="B79" s="9"/>
-      <c r="C79" s="9"/>
-      <c r="D79" s="9"/>
-      <c r="E79" s="9"/>
-      <c r="F79" s="9"/>
-      <c r="G79" s="9"/>
-      <c r="H79" s="9"/>
-      <c r="I79" s="12"/>
+      <c r="B79" s="20"/>
+      <c r="C79" s="20"/>
+      <c r="D79" s="20"/>
+      <c r="E79" s="20"/>
+      <c r="F79" s="20"/>
+      <c r="G79" s="20"/>
+      <c r="H79" s="20"/>
+      <c r="I79" s="10"/>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A80" s="3"/>
-      <c r="B80" s="9"/>
-      <c r="C80" s="9"/>
-      <c r="D80" s="9"/>
-      <c r="E80" s="9"/>
-      <c r="F80" s="9"/>
-      <c r="G80" s="9"/>
-      <c r="H80" s="9"/>
-      <c r="I80" s="12"/>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="B80" s="20"/>
+      <c r="C80" s="20"/>
+      <c r="D80" s="20"/>
+      <c r="E80" s="20"/>
+      <c r="F80" s="20"/>
+      <c r="G80" s="20"/>
+      <c r="H80" s="20"/>
+      <c r="I80" s="10"/>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A81" s="3"/>
-      <c r="B81" s="9"/>
-      <c r="C81" s="9"/>
-      <c r="D81" s="9"/>
-      <c r="E81" s="9"/>
-      <c r="F81" s="9"/>
-      <c r="G81" s="9"/>
-      <c r="H81" s="9"/>
-      <c r="I81" s="12"/>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="B81" s="20"/>
+      <c r="C81" s="20"/>
+      <c r="D81" s="20"/>
+      <c r="E81" s="20"/>
+      <c r="F81" s="20"/>
+      <c r="G81" s="20"/>
+      <c r="H81" s="20"/>
+      <c r="I81" s="10"/>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A82" s="3"/>
-      <c r="B82" s="9"/>
-      <c r="C82" s="9"/>
-      <c r="D82" s="9"/>
-      <c r="E82" s="9"/>
-      <c r="F82" s="9"/>
-      <c r="G82" s="9"/>
-      <c r="H82" s="9"/>
-      <c r="I82" s="12"/>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="B82" s="20"/>
+      <c r="C82" s="20"/>
+      <c r="D82" s="20"/>
+      <c r="E82" s="20"/>
+      <c r="F82" s="20"/>
+      <c r="G82" s="20"/>
+      <c r="H82" s="20"/>
+      <c r="I82" s="10"/>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A83" s="3"/>
-      <c r="B83" s="9"/>
-      <c r="C83" s="9"/>
-      <c r="D83" s="9"/>
-      <c r="E83" s="9"/>
-      <c r="F83" s="9"/>
-      <c r="G83" s="9"/>
-      <c r="H83" s="9"/>
-      <c r="I83" s="12"/>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="B83" s="20"/>
+      <c r="C83" s="20"/>
+      <c r="D83" s="20"/>
+      <c r="E83" s="20"/>
+      <c r="F83" s="20"/>
+      <c r="G83" s="20"/>
+      <c r="H83" s="20"/>
+      <c r="I83" s="10"/>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A84" s="3"/>
-      <c r="B84" s="9"/>
-      <c r="C84" s="9"/>
-      <c r="D84" s="9"/>
-      <c r="E84" s="9"/>
-      <c r="F84" s="9"/>
-      <c r="G84" s="9"/>
-      <c r="H84" s="9"/>
-      <c r="I84" s="12"/>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="B84" s="20"/>
+      <c r="C84" s="20"/>
+      <c r="D84" s="20"/>
+      <c r="E84" s="20"/>
+      <c r="F84" s="20"/>
+      <c r="G84" s="20"/>
+      <c r="H84" s="20"/>
+      <c r="I84" s="10"/>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A85" s="4"/>
-      <c r="B85" s="10"/>
-      <c r="C85" s="10"/>
-      <c r="D85" s="10"/>
-      <c r="E85" s="10"/>
-      <c r="F85" s="10"/>
-      <c r="G85" s="10"/>
-      <c r="H85" s="10"/>
-      <c r="I85" s="13"/>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A86" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B86" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C86" s="8"/>
-      <c r="D86" s="8"/>
-      <c r="E86" s="8"/>
-      <c r="F86" s="8"/>
-      <c r="G86" s="8"/>
-      <c r="H86" s="8"/>
-      <c r="I86" s="11"/>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A87" s="3"/>
-      <c r="B87" s="9"/>
-      <c r="C87" s="9"/>
-      <c r="D87" s="9"/>
-      <c r="E87" s="9"/>
-      <c r="F87" s="9"/>
-      <c r="G87" s="9"/>
-      <c r="H87" s="9"/>
-      <c r="I87" s="12"/>
-    </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A88" s="3"/>
-      <c r="B88" s="9"/>
-      <c r="C88" s="9"/>
-      <c r="D88" s="9"/>
-      <c r="E88" s="9"/>
-      <c r="F88" s="9"/>
-      <c r="G88" s="9"/>
-      <c r="H88" s="9"/>
-      <c r="I88" s="12"/>
-    </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A89" s="3"/>
-      <c r="B89" s="9"/>
-      <c r="C89" s="9"/>
-      <c r="D89" s="9"/>
-      <c r="E89" s="9"/>
-      <c r="F89" s="9"/>
-      <c r="G89" s="9"/>
-      <c r="H89" s="9"/>
-      <c r="I89" s="12"/>
-    </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A90" s="3"/>
-      <c r="B90" s="9"/>
-      <c r="C90" s="9"/>
-      <c r="D90" s="9"/>
-      <c r="E90" s="9"/>
-      <c r="F90" s="9"/>
-      <c r="G90" s="9"/>
-      <c r="H90" s="9"/>
-      <c r="I90" s="12"/>
-    </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A91" s="3"/>
-      <c r="B91" s="9"/>
-      <c r="C91" s="9"/>
-      <c r="D91" s="9"/>
-      <c r="E91" s="9"/>
-      <c r="F91" s="9"/>
-      <c r="G91" s="9"/>
-      <c r="H91" s="9"/>
-      <c r="I91" s="12"/>
-    </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A92" s="3"/>
-      <c r="B92" s="9"/>
-      <c r="C92" s="9"/>
-      <c r="D92" s="9"/>
-      <c r="E92" s="9"/>
-      <c r="F92" s="9"/>
-      <c r="G92" s="9"/>
-      <c r="H92" s="9"/>
-      <c r="I92" s="12"/>
-    </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A93" s="3"/>
-      <c r="B93" s="9"/>
-      <c r="C93" s="9"/>
-      <c r="D93" s="9"/>
-      <c r="E93" s="9"/>
-      <c r="F93" s="9"/>
-      <c r="G93" s="9"/>
-      <c r="H93" s="9"/>
-      <c r="I93" s="12"/>
-    </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A94" s="4"/>
-      <c r="B94" s="10"/>
-      <c r="C94" s="10"/>
-      <c r="D94" s="10"/>
-      <c r="E94" s="10"/>
-      <c r="F94" s="10"/>
-      <c r="G94" s="10"/>
-      <c r="H94" s="10"/>
-      <c r="I94" s="13"/>
+      <c r="B85" s="7"/>
+      <c r="C85" s="7"/>
+      <c r="D85" s="7"/>
+      <c r="E85" s="7"/>
+      <c r="F85" s="7"/>
+      <c r="G85" s="7"/>
+      <c r="H85" s="7"/>
+      <c r="I85" s="11"/>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A86" s="19"/>
+      <c r="B86" s="21"/>
+      <c r="C86" s="19"/>
+      <c r="D86" s="19"/>
+      <c r="E86" s="19"/>
+      <c r="F86" s="19"/>
+      <c r="G86" s="19"/>
+      <c r="H86" s="19"/>
+      <c r="I86" s="19"/>
+      <c r="J86" s="18"/>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A87" s="19"/>
+      <c r="B87" s="19"/>
+      <c r="C87" s="19"/>
+      <c r="D87" s="19"/>
+      <c r="E87" s="19"/>
+      <c r="F87" s="19"/>
+      <c r="G87" s="19"/>
+      <c r="H87" s="19"/>
+      <c r="I87" s="19"/>
+      <c r="J87" s="18"/>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A88" s="19"/>
+      <c r="B88" s="19"/>
+      <c r="C88" s="19"/>
+      <c r="D88" s="19"/>
+      <c r="E88" s="19"/>
+      <c r="F88" s="19"/>
+      <c r="G88" s="19"/>
+      <c r="H88" s="19"/>
+      <c r="I88" s="19"/>
+      <c r="J88" s="18"/>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A89" s="19"/>
+      <c r="B89" s="19"/>
+      <c r="C89" s="19"/>
+      <c r="D89" s="19"/>
+      <c r="E89" s="19"/>
+      <c r="F89" s="19"/>
+      <c r="G89" s="19"/>
+      <c r="H89" s="19"/>
+      <c r="I89" s="19"/>
+      <c r="J89" s="18"/>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A90" s="19"/>
+      <c r="B90" s="19"/>
+      <c r="C90" s="19"/>
+      <c r="D90" s="19"/>
+      <c r="E90" s="19"/>
+      <c r="F90" s="19"/>
+      <c r="G90" s="19"/>
+      <c r="H90" s="19"/>
+      <c r="I90" s="19"/>
+      <c r="J90" s="18"/>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A91" s="19"/>
+      <c r="B91" s="19"/>
+      <c r="C91" s="19"/>
+      <c r="D91" s="19"/>
+      <c r="E91" s="19"/>
+      <c r="F91" s="19"/>
+      <c r="G91" s="19"/>
+      <c r="H91" s="19"/>
+      <c r="I91" s="19"/>
+      <c r="J91" s="18"/>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A92" s="19"/>
+      <c r="B92" s="19"/>
+      <c r="C92" s="19"/>
+      <c r="D92" s="19"/>
+      <c r="E92" s="19"/>
+      <c r="F92" s="19"/>
+      <c r="G92" s="19"/>
+      <c r="H92" s="19"/>
+      <c r="I92" s="19"/>
+      <c r="J92" s="18"/>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A93" s="19"/>
+      <c r="B93" s="19"/>
+      <c r="C93" s="19"/>
+      <c r="D93" s="19"/>
+      <c r="E93" s="19"/>
+      <c r="F93" s="19"/>
+      <c r="G93" s="19"/>
+      <c r="H93" s="19"/>
+      <c r="I93" s="19"/>
+      <c r="J93" s="18"/>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A94" s="19"/>
+      <c r="B94" s="19"/>
+      <c r="C94" s="19"/>
+      <c r="D94" s="19"/>
+      <c r="E94" s="19"/>
+      <c r="F94" s="19"/>
+      <c r="G94" s="19"/>
+      <c r="H94" s="19"/>
+      <c r="I94" s="19"/>
+      <c r="J94" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="53">
-    <mergeCell ref="A86:A94"/>
-    <mergeCell ref="B86:B94"/>
-    <mergeCell ref="C86:C94"/>
-    <mergeCell ref="D86:F94"/>
-    <mergeCell ref="G86:I94"/>
-    <mergeCell ref="A77:A85"/>
-    <mergeCell ref="B77:B85"/>
-    <mergeCell ref="C77:C85"/>
-    <mergeCell ref="D77:F85"/>
-    <mergeCell ref="G77:I85"/>
-    <mergeCell ref="A68:A76"/>
-    <mergeCell ref="B68:B76"/>
-    <mergeCell ref="C68:C76"/>
-    <mergeCell ref="D68:F76"/>
-    <mergeCell ref="G68:I76"/>
-    <mergeCell ref="A59:A67"/>
-    <mergeCell ref="B59:B67"/>
-    <mergeCell ref="C59:C67"/>
-    <mergeCell ref="D59:F67"/>
-    <mergeCell ref="G59:I67"/>
-    <mergeCell ref="A41:A49"/>
-    <mergeCell ref="B41:B49"/>
-    <mergeCell ref="C41:C49"/>
-    <mergeCell ref="D41:F49"/>
-    <mergeCell ref="G41:I49"/>
-    <mergeCell ref="A32:A40"/>
-    <mergeCell ref="B32:B40"/>
-    <mergeCell ref="C32:C40"/>
-    <mergeCell ref="D32:F40"/>
-    <mergeCell ref="G32:I40"/>
+  <mergeCells count="48">
+    <mergeCell ref="A50:A58"/>
+    <mergeCell ref="B50:B58"/>
+    <mergeCell ref="C50:C58"/>
+    <mergeCell ref="D50:F58"/>
+    <mergeCell ref="G50:I58"/>
+    <mergeCell ref="A23:A31"/>
+    <mergeCell ref="B23:B31"/>
+    <mergeCell ref="C23:C31"/>
+    <mergeCell ref="D23:F31"/>
+    <mergeCell ref="G23:I31"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="A5:A13"/>
+    <mergeCell ref="B5:B13"/>
+    <mergeCell ref="C5:C13"/>
     <mergeCell ref="G4:I4"/>
     <mergeCell ref="D5:F13"/>
     <mergeCell ref="G5:I13"/>
@@ -3866,21 +5093,31 @@
     <mergeCell ref="C14:C22"/>
     <mergeCell ref="D14:F22"/>
     <mergeCell ref="G14:I22"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="A5:A13"/>
-    <mergeCell ref="B5:B13"/>
-    <mergeCell ref="C5:C13"/>
-    <mergeCell ref="A23:A31"/>
-    <mergeCell ref="B23:B31"/>
-    <mergeCell ref="C23:C31"/>
-    <mergeCell ref="D23:F31"/>
-    <mergeCell ref="G23:I31"/>
-    <mergeCell ref="A50:A58"/>
-    <mergeCell ref="B50:B58"/>
-    <mergeCell ref="C50:C58"/>
-    <mergeCell ref="D50:F58"/>
-    <mergeCell ref="G50:I58"/>
+    <mergeCell ref="A32:A40"/>
+    <mergeCell ref="B32:B40"/>
+    <mergeCell ref="C32:C40"/>
+    <mergeCell ref="D32:F40"/>
+    <mergeCell ref="G32:I40"/>
+    <mergeCell ref="A41:A49"/>
+    <mergeCell ref="B41:B49"/>
+    <mergeCell ref="C41:C49"/>
+    <mergeCell ref="D41:F49"/>
+    <mergeCell ref="G41:I49"/>
+    <mergeCell ref="A59:A67"/>
+    <mergeCell ref="B59:B67"/>
+    <mergeCell ref="C59:C67"/>
+    <mergeCell ref="D59:F67"/>
+    <mergeCell ref="G59:I67"/>
+    <mergeCell ref="A68:A76"/>
+    <mergeCell ref="B68:B76"/>
+    <mergeCell ref="C68:C76"/>
+    <mergeCell ref="D68:F76"/>
+    <mergeCell ref="G68:I76"/>
+    <mergeCell ref="A77:A85"/>
+    <mergeCell ref="B77:B85"/>
+    <mergeCell ref="C77:C85"/>
+    <mergeCell ref="D77:F85"/>
+    <mergeCell ref="G77:I85"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3888,7 +5125,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78D24CAE-E098-47FA-9D18-51E847D08958}">
   <dimension ref="L1:O119"/>
   <sheetViews>
@@ -5505,7 +6742,7 @@
     </row>
     <row r="102" spans="12:15" x14ac:dyDescent="0.45">
       <c r="L102" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M102">
         <v>0.453125</v>
@@ -5521,7 +6758,7 @@
     </row>
     <row r="103" spans="12:15" x14ac:dyDescent="0.45">
       <c r="L103" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M103">
         <v>0.625</v>
@@ -5537,7 +6774,7 @@
     </row>
     <row r="104" spans="12:15" x14ac:dyDescent="0.45">
       <c r="L104" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M104">
         <v>0.40625</v>
@@ -5553,7 +6790,7 @@
     </row>
     <row r="105" spans="12:15" x14ac:dyDescent="0.45">
       <c r="L105" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M105">
         <v>0.5625</v>
@@ -5569,7 +6806,7 @@
     </row>
     <row r="106" spans="12:15" x14ac:dyDescent="0.45">
       <c r="L106" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M106">
         <v>0.484375</v>
@@ -5585,7 +6822,7 @@
     </row>
     <row r="107" spans="12:15" x14ac:dyDescent="0.45">
       <c r="L107" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M107">
         <v>0.390625</v>
@@ -5601,7 +6838,7 @@
     </row>
     <row r="108" spans="12:15" x14ac:dyDescent="0.45">
       <c r="L108" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M108">
         <v>0.546875</v>
@@ -5617,7 +6854,7 @@
     </row>
     <row r="109" spans="12:15" x14ac:dyDescent="0.45">
       <c r="L109" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M109">
         <v>0.546875</v>
@@ -5633,7 +6870,7 @@
     </row>
     <row r="110" spans="12:15" x14ac:dyDescent="0.45">
       <c r="L110" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M110">
         <v>0.515625</v>
@@ -5649,7 +6886,7 @@
     </row>
     <row r="111" spans="12:15" x14ac:dyDescent="0.45">
       <c r="L111" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M111">
         <v>0.5</v>
@@ -5665,7 +6902,7 @@
     </row>
     <row r="112" spans="12:15" x14ac:dyDescent="0.45">
       <c r="L112" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M112">
         <v>0.453125</v>
@@ -5681,7 +6918,7 @@
     </row>
     <row r="113" spans="12:15" x14ac:dyDescent="0.45">
       <c r="L113" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M113">
         <v>0.5625</v>
@@ -5697,7 +6934,7 @@
     </row>
     <row r="114" spans="12:15" x14ac:dyDescent="0.45">
       <c r="L114" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M114">
         <v>0.40625</v>
@@ -5713,7 +6950,7 @@
     </row>
     <row r="115" spans="12:15" x14ac:dyDescent="0.45">
       <c r="L115" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M115">
         <v>0.53125</v>
@@ -5729,7 +6966,7 @@
     </row>
     <row r="116" spans="12:15" x14ac:dyDescent="0.45">
       <c r="L116" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M116">
         <v>0.46875</v>
@@ -5745,7 +6982,7 @@
     </row>
     <row r="117" spans="12:15" x14ac:dyDescent="0.45">
       <c r="L117" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M117">
         <v>0.453125</v>
@@ -5761,7 +6998,7 @@
     </row>
     <row r="118" spans="12:15" x14ac:dyDescent="0.45">
       <c r="L118" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M118">
         <v>0.57377049180327866</v>

</xml_diff>